<commit_message>
pixmosaic with video from youtube
</commit_message>
<xml_diff>
--- a/storage/app/import/pixmosaic-video/pix_video.xlsx
+++ b/storage/app/import/pixmosaic-video/pix_video.xlsx
@@ -717,334 +717,334 @@
     <t>PIX766</t>
   </si>
   <si>
-    <t>https://www.youtube.com/shorts/D4rlWGFGbds</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/dPQXL9jaHc0</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/6Z3MzD68am4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/3q04M_Gsq0s</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/mXBZArss4Y4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/5O_xfnVw-bA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/fhkddsgy8OU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/sixQRSszrEg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/xtcdZBYjhxc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/kaLq-mEoCm0</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/0Xt-3h8FGn4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/1vCkpDxnlT4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/W3rI-lxD5wE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/XSQ-ZlxYqeg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/dR-94tc5VHg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/ocxTqZDuEzA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/pGo0BhkNenY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/ptKmppo6DIU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/sSBrQ0_IwcU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/-tcQ809zi8k</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/RBPqpkTfHzE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/RpoaRmDfQDs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/dpOdrRP4rrY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/eW-MDtAUF_Q</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/g58G4bEfojc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/7VwVbAE9lTY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/BAhXXgveWK0</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/G-RpokuJppw</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/IFDzGkNvPFs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/JfmgBo46QjY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/iUllStdPS4s</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/lu5H26h9Ll0</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/z7KqaCM3Q9E</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/2KdBMpGDRGI</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/4bSnlTaWR-0</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/PLmOjJB4G8o</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/aBt81q9Q4x8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/aoBjLIn4PiM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/e5Nc8wziKIc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/fY1eNOamFZw</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/y8GFjkg9Cqs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/2rT4pWThBKs</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/Ba0HsJKFVZM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/Dnm0x0SKN6g</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/LYJK-K7PrtM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/kSP-bbzEj7g</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/m3UeuBXHOGo</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/qjSZsM0WSX0</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/uFK8p1zreBU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/v_d4QWKy4xY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/YkHBJDNj6dU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/a-w878fSfvM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/cTuB1hFB5EA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/iOOQ8MA57Ow</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/jbyGZVYT3oM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/u5eTqV1iqzE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/6Nti4_4CNYA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/OIKyPQaBGCw</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/QHm6qySAqSk</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/XtKamuaOpQY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/lWqa2JQRyEM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/mKiahKFh4ns</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/qqOC0EYhZmA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/tiukuAudKRg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/tz3vCzsSnZc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/TBU1vyaMavQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/UEFUF9Vk9Cc</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/Z70T3nlLoGA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/bSuUDPCHZWM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/fMvCnZlGkEQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/CBKjfcNNR44</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/CEZ3NnhNqNI</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/GO0c6WvdxXQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/OICvSJtWHC0</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/Qlwkpj7dHMY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/CsNyfaIasvk</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/GxE_dXSiN00</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=QwK1fpLL2jE&amp;ab_channel=PixelMosaic</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/hPLscZkCREg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/zzjzvf8riGA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/SReZkkgG-WM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/Z_0EQMYjd_Y</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/rOK7_ZjBtlk</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/6-EQO_LoYM8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/COI_pNBQnDA</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/hHJVYGzjjJQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=rwbaTwRAsYg&amp;ab_channel=PixelMosaic</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/2PnKw3gwjsw</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/IF5VbdKzAJQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=NKnBXA1f1vs&amp;ab_channel=PixelMosaic</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/liH2Dy-8KNE</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/8fsTW-Q15a8</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/AqGGozuyfZ4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/yH4zzl25NMk</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/XxkrL22VhtQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/watch?v=u11hA-XiLpE&amp;ab_channel=PixelMosaic</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/KD7vjf82EOM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/QJV5Kd8-4_E</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/BILdIQNaLYU</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/CnuyKDF7Vms</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/9KpjUaFwuic</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/TMsbAHA9YSo</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/KKSI4V9m6_4</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/eIwq6TucEIM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/y1mou-NjmCg</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/NypuYkkk6FY</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/Lq6xJM3J2UQ</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/tb90n3dqVkM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/7Uyz5ytknXM</t>
-  </si>
-  <si>
-    <t>https://www.youtube.com/shorts/zxglCzNS1Ag</t>
+    <t>https://www.youtube.com/watch?v=u11hA-XiLpE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QwK1fpLL2jE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rwbaTwRAsYg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=NKnBXA1f1vs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=RBPqpkTfHzE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=aoBjLIn4PiM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fY1eNOamFZw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=eW-MDtAUF_Q</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=4bSnlTaWR-0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7VwVbAE9lTY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=-tcQ809zi8k</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lu5H26h9Ll0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=IFDzGkNvPFs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XtKamuaOpQY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dR-94tc5VHg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dpOdrRP4rrY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hPLscZkCREg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kaLq-mEoCm0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=G-RpokuJppw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1vCkpDxnlT4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=W3rI-lxD5wE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=0Xt-3h8FGn4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ptKmppo6DIU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=kSP-bbzEj7g</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=COI_pNBQnDA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XSQ-ZlxYqeg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CBKjfcNNR44</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=dPQXL9jaHc0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=y8GFjkg9Cqs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=SReZkkgG-WM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GxE_dXSiN00</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=IF5VbdKzAJQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=y1mou-NjmCg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=eIwq6TucEIM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=KKSI4V9m6_4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zxglCzNS1Ag</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=7Uyz5ytknXM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=tb90n3dqVkM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Lq6xJM3J2UQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=NypuYkkk6FY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=aBt81q9Q4x8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Z_0EQMYjd_Y</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2KdBMpGDRGI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=jbyGZVYT3oM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=tiukuAudKRg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CEZ3NnhNqNI</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=uFK8p1zreBU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sixQRSszrEg</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Z70T3nlLoGA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=BILdIQNaLYU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=mXBZArss4Y4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XxkrL22VhtQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=KD7vjf82EOM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=5O_xfnVw-bA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=TBU1vyaMavQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=bSuUDPCHZWM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=m3UeuBXHOGo</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=pGo0BhkNenY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=JfmgBo46QjY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=xtcdZBYjhxc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cTuB1hFB5EA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=mKiahKFh4ns</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=z7KqaCM3Q9E</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=rOK7_ZjBtlk</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=g58G4bEfojc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=D4rlWGFGbds</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CnuyKDF7Vms</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=LYJK-K7PrtM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CsNyfaIasvk</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=8fsTW-Q15a8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QJV5Kd8-4_E</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=v_d4QWKy4xY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=YkHBJDNj6dU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=OICvSJtWHC0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ocxTqZDuEzA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fhkddsgy8OU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=a-w878fSfvM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=u5eTqV1iqzE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qqOC0EYhZmA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=RpoaRmDfQDs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=yH4zzl25NMk</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=UEFUF9Vk9Cc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=liH2Dy-8KNE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=AqGGozuyfZ4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=TMsbAHA9YSo</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6Nti4_4CNYA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6-EQO_LoYM8</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=sSBrQ0_IwcU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=BAhXXgveWK0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=lWqa2JQRyEM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6Z3MzD68am4</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2PnKw3gwjsw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=9KpjUaFwuic</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=fMvCnZlGkEQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=hHJVYGzjjJQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qjSZsM0WSX0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Qlwkpj7dHMY</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GO0c6WvdxXQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=QHm6qySAqSk</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=OIKyPQaBGCw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=tz3vCzsSnZc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Dnm0x0SKN6g</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2rT4pWThBKs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=zzjzvf8riGA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PLmOjJB4G8o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=3q04M_Gsq0s</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Ba0HsJKFVZM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=e5Nc8wziKIc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=iOOQ8MA57Ow</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=iUllStdPS4s</t>
   </si>
 </sst>
 </file>
@@ -1395,7 +1395,7 @@
   <dimension ref="A1:B232"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1417,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1435,7 +1435,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>270</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1443,7 +1443,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>272</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1451,7 +1451,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1459,7 +1459,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>267</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1467,15 +1467,15 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
-        <v>252</v>
+      <c r="B10" s="2" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1483,7 +1483,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>264</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1491,7 +1491,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1504,7 +1504,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>292</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1520,7 +1520,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1528,7 +1528,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>311</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1536,7 +1536,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>242</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1544,7 +1544,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1552,7 +1552,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1560,7 +1560,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>245</v>
+        <v>253</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1568,7 +1568,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1576,7 +1576,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1584,7 +1584,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1592,7 +1592,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>317</v>
+        <v>257</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1600,7 +1600,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1608,7 +1608,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>303</v>
+        <v>259</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1616,7 +1616,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>234</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1654,7 +1654,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -1662,7 +1662,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>313</v>
+        <v>262</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -1670,7 +1670,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>309</v>
+        <v>263</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -1678,7 +1678,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>321</v>
+        <v>264</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -1696,7 +1696,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>337</v>
+        <v>265</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -1719,7 +1719,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>336</v>
+        <v>266</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -1727,7 +1727,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>335</v>
+        <v>267</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -1735,7 +1735,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>342</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -1858,7 +1858,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>341</v>
+        <v>269</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -1866,7 +1866,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>340</v>
+        <v>270</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -1874,7 +1874,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>339</v>
+        <v>271</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -1902,7 +1902,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>338</v>
+        <v>272</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1920,7 +1920,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1928,7 +1928,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>314</v>
+        <v>274</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -1936,7 +1936,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -1944,7 +1944,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2017,7 +2017,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2025,7 +2025,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>304</v>
+        <v>278</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2033,7 +2033,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2041,7 +2041,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>240</v>
+        <v>280</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2049,7 +2049,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>300</v>
+        <v>281</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2057,7 +2057,7 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>331</v>
+        <v>282</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2065,7 +2065,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>237</v>
+        <v>283</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2073,7 +2073,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>327</v>
+        <v>284</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2081,7 +2081,7 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>329</v>
+        <v>285</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2089,7 +2089,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>238</v>
+        <v>286</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2102,7 +2102,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2130,7 +2130,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -2138,7 +2138,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -2146,7 +2146,7 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>249</v>
+        <v>290</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -2154,7 +2154,7 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>262</v>
+        <v>291</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -2162,7 +2162,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>241</v>
+        <v>292</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -2170,7 +2170,7 @@
         <v>119</v>
       </c>
       <c r="B119" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -2261,7 +2261,7 @@
         <v>136</v>
       </c>
       <c r="B136" t="s">
-        <v>265</v>
+        <v>295</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -2269,7 +2269,7 @@
         <v>137</v>
       </c>
       <c r="B137" t="s">
-        <v>315</v>
+        <v>296</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -2277,7 +2277,7 @@
         <v>138</v>
       </c>
       <c r="B138" t="s">
-        <v>257</v>
+        <v>297</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -2285,7 +2285,7 @@
         <v>139</v>
       </c>
       <c r="B139" t="s">
-        <v>233</v>
+        <v>298</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2297,8 +2297,8 @@
       <c r="A141" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B141" t="s">
-        <v>328</v>
+      <c r="B141" s="2" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2306,7 +2306,7 @@
         <v>142</v>
       </c>
       <c r="B142" t="s">
-        <v>332</v>
+        <v>299</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2314,15 +2314,15 @@
         <v>143</v>
       </c>
       <c r="B143" t="s">
-        <v>277</v>
+        <v>300</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B144" t="s">
-        <v>310</v>
+      <c r="B144" s="2" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -2330,7 +2330,7 @@
         <v>145</v>
       </c>
       <c r="B145" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -2338,7 +2338,7 @@
         <v>146</v>
       </c>
       <c r="B146" t="s">
-        <v>324</v>
+        <v>302</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -2351,7 +2351,7 @@
         <v>148</v>
       </c>
       <c r="B148" t="s">
-        <v>330</v>
+        <v>303</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -2359,7 +2359,7 @@
         <v>149</v>
       </c>
       <c r="B149" t="s">
-        <v>282</v>
+        <v>304</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2372,7 +2372,7 @@
         <v>151</v>
       </c>
       <c r="B151" t="s">
-        <v>283</v>
+        <v>305</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -2403,7 +2403,7 @@
         <v>156</v>
       </c>
       <c r="B156" t="s">
-        <v>248</v>
+        <v>307</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -2411,7 +2411,7 @@
         <v>157</v>
       </c>
       <c r="B157" t="s">
-        <v>239</v>
+        <v>308</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -2419,7 +2419,7 @@
         <v>158</v>
       </c>
       <c r="B158" t="s">
-        <v>284</v>
+        <v>309</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2427,7 +2427,7 @@
         <v>159</v>
       </c>
       <c r="B159" t="s">
-        <v>288</v>
+        <v>310</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2440,7 +2440,7 @@
         <v>161</v>
       </c>
       <c r="B161" t="s">
-        <v>295</v>
+        <v>311</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2448,7 +2448,7 @@
         <v>162</v>
       </c>
       <c r="B162" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2491,7 +2491,7 @@
         <v>170</v>
       </c>
       <c r="B170" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
     </row>
     <row r="171" spans="1:2">
@@ -2538,8 +2538,8 @@
       <c r="A179" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="B179" t="s">
-        <v>319</v>
+      <c r="B179" s="2" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="180" spans="1:2">
@@ -2552,7 +2552,7 @@
         <v>181</v>
       </c>
       <c r="B181" t="s">
-        <v>299</v>
+        <v>314</v>
       </c>
     </row>
     <row r="182" spans="1:2">
@@ -2565,7 +2565,7 @@
         <v>183</v>
       </c>
       <c r="B183" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
     </row>
     <row r="184" spans="1:2">
@@ -2573,7 +2573,7 @@
         <v>184</v>
       </c>
       <c r="B184" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="185" spans="1:2">
@@ -2581,7 +2581,7 @@
         <v>185</v>
       </c>
       <c r="B185" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
     </row>
     <row r="186" spans="1:2">
@@ -2589,7 +2589,7 @@
         <v>186</v>
       </c>
       <c r="B186" t="s">
-        <v>289</v>
+        <v>318</v>
       </c>
     </row>
     <row r="187" spans="1:2">
@@ -2597,7 +2597,7 @@
         <v>187</v>
       </c>
       <c r="B187" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
     </row>
     <row r="188" spans="1:2">
@@ -2605,15 +2605,15 @@
         <v>188</v>
       </c>
       <c r="B188" t="s">
-        <v>251</v>
+        <v>320</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B189" t="s">
-        <v>259</v>
+      <c r="B189" s="2" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="190" spans="1:2">
@@ -2621,7 +2621,7 @@
         <v>190</v>
       </c>
       <c r="B190" t="s">
-        <v>293</v>
+        <v>322</v>
       </c>
     </row>
     <row r="191" spans="1:2">
@@ -2629,7 +2629,7 @@
         <v>191</v>
       </c>
       <c r="B191" t="s">
-        <v>235</v>
+        <v>323</v>
       </c>
     </row>
     <row r="192" spans="1:2">
@@ -2642,7 +2642,7 @@
         <v>193</v>
       </c>
       <c r="B193" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
     </row>
     <row r="194" spans="1:2">
@@ -2650,7 +2650,7 @@
         <v>194</v>
       </c>
       <c r="B194" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="195" spans="1:2">
@@ -2658,7 +2658,7 @@
         <v>195</v>
       </c>
       <c r="B195" t="s">
-        <v>302</v>
+        <v>326</v>
       </c>
     </row>
     <row r="196" spans="1:2">
@@ -2671,7 +2671,7 @@
         <v>197</v>
       </c>
       <c r="B197" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
     </row>
     <row r="198" spans="1:2">
@@ -2679,7 +2679,7 @@
         <v>198</v>
       </c>
       <c r="B198" t="s">
-        <v>280</v>
+        <v>328</v>
       </c>
     </row>
     <row r="199" spans="1:2">
@@ -2687,15 +2687,15 @@
         <v>199</v>
       </c>
       <c r="B199" t="s">
-        <v>307</v>
+        <v>329</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B200" t="s">
-        <v>305</v>
+      <c r="B200" s="2" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="201" spans="1:2">
@@ -2708,7 +2708,7 @@
         <v>202</v>
       </c>
       <c r="B202" t="s">
-        <v>291</v>
+        <v>331</v>
       </c>
     </row>
     <row r="203" spans="1:2">
@@ -2716,7 +2716,7 @@
         <v>203</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>322</v>
+        <v>236</v>
       </c>
     </row>
     <row r="204" spans="1:2">
@@ -2739,7 +2739,7 @@
         <v>207</v>
       </c>
       <c r="B207" t="s">
-        <v>290</v>
+        <v>332</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2747,7 +2747,7 @@
         <v>208</v>
       </c>
       <c r="B208" t="s">
-        <v>297</v>
+        <v>333</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2755,7 +2755,7 @@
         <v>209</v>
       </c>
       <c r="B209" t="s">
-        <v>276</v>
+        <v>334</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2763,7 +2763,7 @@
         <v>210</v>
       </c>
       <c r="B210" t="s">
-        <v>274</v>
+        <v>335</v>
       </c>
     </row>
     <row r="211" spans="1:2">
@@ -2771,7 +2771,7 @@
         <v>211</v>
       </c>
       <c r="B211" t="s">
-        <v>312</v>
+        <v>336</v>
       </c>
     </row>
     <row r="212" spans="1:2">
@@ -2779,7 +2779,7 @@
         <v>212</v>
       </c>
       <c r="B212" t="s">
-        <v>268</v>
+        <v>337</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2802,7 +2802,7 @@
         <v>216</v>
       </c>
       <c r="B216" t="s">
-        <v>236</v>
+        <v>338</v>
       </c>
     </row>
     <row r="217" spans="1:2">
@@ -2810,7 +2810,7 @@
         <v>217</v>
       </c>
       <c r="B217" t="s">
-        <v>275</v>
+        <v>339</v>
       </c>
     </row>
     <row r="218" spans="1:2">
@@ -2818,7 +2818,7 @@
         <v>218</v>
       </c>
       <c r="B218" t="s">
-        <v>271</v>
+        <v>340</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2826,7 +2826,7 @@
         <v>219</v>
       </c>
       <c r="B219" t="s">
-        <v>286</v>
+        <v>341</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2834,7 +2834,7 @@
         <v>220</v>
       </c>
       <c r="B220" t="s">
-        <v>263</v>
+        <v>342</v>
       </c>
     </row>
     <row r="221" spans="1:2">
@@ -2900,9 +2900,15 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B203" r:id="rId1"/>
+    <hyperlink ref="B141" r:id="rId2"/>
+    <hyperlink ref="B144" r:id="rId3"/>
+    <hyperlink ref="B179" r:id="rId4"/>
+    <hyperlink ref="B200" r:id="rId5" display="https://www.youtube.com/shorts/GO0c6WvdxXQ"/>
+    <hyperlink ref="B189" r:id="rId6"/>
+    <hyperlink ref="B10" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
pixmosaic new video 2
</commit_message>
<xml_diff>
--- a/storage/app/import/pixmosaic-video/pix_video.xlsx
+++ b/storage/app/import/pixmosaic-video/pix_video.xlsx
@@ -1266,9 +1266,6 @@
     <t>PIX332</t>
   </si>
   <si>
-    <t>PIX339</t>
-  </si>
-  <si>
     <t>PIX330</t>
   </si>
   <si>
@@ -1414,6 +1411,9 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=A2Oe2ouYu9w</t>
+  </si>
+  <si>
+    <t>PIX329</t>
   </si>
 </sst>
 </file>
@@ -1763,8 +1763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
+    <sheetView tabSelected="1" topLeftCell="A126" workbookViewId="0">
+      <selection activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2733,114 +2733,114 @@
     </row>
     <row r="126" spans="1:2">
       <c r="A126" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" s="1" t="s">
-        <v>417</v>
+        <v>465</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" s="1" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" s="1" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -2848,7 +2848,7 @@
         <v>429</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -2856,7 +2856,7 @@
         <v>428</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -2864,7 +2864,7 @@
         <v>427</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -2872,23 +2872,23 @@
         <v>426</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" s="1" t="s">
-        <v>414</v>
+        <v>425</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -3584,7 +3584,7 @@
         <v>221</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -3592,7 +3592,7 @@
         <v>222</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="243" spans="1:2">
@@ -3600,7 +3600,7 @@
         <v>223</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="244" spans="1:2">
@@ -3608,7 +3608,7 @@
         <v>224</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="245" spans="1:2">
@@ -3616,7 +3616,7 @@
         <v>225</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="246" spans="1:2">
@@ -3624,7 +3624,7 @@
         <v>226</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="247" spans="1:2">
@@ -3632,7 +3632,7 @@
         <v>227</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="248" spans="1:2">
@@ -3640,7 +3640,7 @@
         <v>228</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="249" spans="1:2">
@@ -3648,7 +3648,7 @@
         <v>229</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="250" spans="1:2">
@@ -3656,7 +3656,7 @@
         <v>230</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="251" spans="1:2">
@@ -3664,7 +3664,7 @@
         <v>231</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="252" spans="1:2">
@@ -3672,7 +3672,7 @@
         <v>232</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
   </sheetData>
@@ -3781,15 +3781,15 @@
     <hyperlink ref="B134" r:id="rId102"/>
     <hyperlink ref="B135" r:id="rId103"/>
     <hyperlink ref="B136" r:id="rId104"/>
-    <hyperlink ref="B137" r:id="rId105"/>
-    <hyperlink ref="B138" r:id="rId106"/>
-    <hyperlink ref="B139" r:id="rId107"/>
-    <hyperlink ref="B140" r:id="rId108"/>
-    <hyperlink ref="B141" r:id="rId109"/>
-    <hyperlink ref="B142" r:id="rId110"/>
-    <hyperlink ref="B143" r:id="rId111"/>
-    <hyperlink ref="B144" r:id="rId112"/>
-    <hyperlink ref="B145" r:id="rId113"/>
+    <hyperlink ref="B138" r:id="rId105"/>
+    <hyperlink ref="B139" r:id="rId106"/>
+    <hyperlink ref="B140" r:id="rId107"/>
+    <hyperlink ref="B141" r:id="rId108"/>
+    <hyperlink ref="B142" r:id="rId109"/>
+    <hyperlink ref="B143" r:id="rId110"/>
+    <hyperlink ref="B144" r:id="rId111"/>
+    <hyperlink ref="B145" r:id="rId112"/>
+    <hyperlink ref="B137" r:id="rId113"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId114"/>

</xml_diff>